<commit_message>
Added j:PersonRaceCode and disp-ext:RecidivismEligibilityDate to the Vermont Dispo Report.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Codes.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Codes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="19425" windowHeight="13065" tabRatio="771" firstSheet="1" activeTab="15"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="19425" windowHeight="13065" tabRatio="771" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="OffLevel" sheetId="4" r:id="rId1"/>
@@ -18,11 +18,10 @@
     <sheet name="PleaChange" sheetId="18" r:id="rId9"/>
     <sheet name="ProDispCode" sheetId="20" r:id="rId10"/>
     <sheet name="PTStat" sheetId="21" r:id="rId11"/>
-    <sheet name="Race" sheetId="22" r:id="rId12"/>
-    <sheet name="SentCat" sheetId="25" r:id="rId13"/>
-    <sheet name="VTRes" sheetId="26" r:id="rId14"/>
-    <sheet name="County" sheetId="27" r:id="rId15"/>
-    <sheet name="Sentence" sheetId="28" r:id="rId16"/>
+    <sheet name="SentCat" sheetId="25" r:id="rId12"/>
+    <sheet name="VTRes" sheetId="26" r:id="rId13"/>
+    <sheet name="County" sheetId="27" r:id="rId14"/>
+    <sheet name="Sentence" sheetId="28" r:id="rId15"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="195">
   <si>
     <t>UNKNOWN</t>
   </si>
@@ -345,33 +344,6 @@
     <t>BAIL ORDERED</t>
   </si>
   <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>African American</t>
-  </si>
-  <si>
-    <t>Asian</t>
-  </si>
-  <si>
-    <t>Caucasian</t>
-  </si>
-  <si>
-    <t>Hispanic</t>
-  </si>
-  <si>
-    <t>Native American</t>
-  </si>
-  <si>
-    <t>Not Reported</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Not Known</t>
-  </si>
-  <si>
     <t>DEATH</t>
   </si>
   <si>
@@ -619,12 +591,6 @@
   </si>
   <si>
     <t>Pre-Trial Status code set</t>
-  </si>
-  <si>
-    <t>RaceCode</t>
-  </si>
-  <si>
-    <t>Race code set</t>
   </si>
   <si>
     <t>SentCatCode</t>
@@ -1155,22 +1121,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -1239,22 +1205,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -1359,22 +1325,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -1450,43 +1416,42 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>103</v>
@@ -1494,7 +1459,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>104</v>
@@ -1502,7 +1467,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>105</v>
@@ -1510,7 +1475,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>106</v>
@@ -1518,7 +1483,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>107</v>
@@ -1526,7 +1491,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>108</v>
@@ -1556,11 +1521,206 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
       <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1578,311 +1738,125 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>130</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>66</v>
-      </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>77</v>
-      </c>
-      <c r="B35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>99</v>
-      </c>
-      <c r="B37" t="s">
-        <v>142</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1903,40 +1877,40 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>143</v>
@@ -1944,7 +1918,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>144</v>
@@ -1952,7 +1926,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>145</v>
@@ -1960,7 +1934,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>146</v>
@@ -1968,7 +1942,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>147</v>
@@ -1976,7 +1950,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>148</v>
@@ -1984,7 +1958,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>149</v>
@@ -1992,7 +1966,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>150</v>
@@ -2000,7 +1974,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>151</v>
@@ -2008,16 +1982,48 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" s="9"/>
     </row>
   </sheetData>
@@ -2039,174 +2045,6 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -2217,22 +2055,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -2242,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2250,7 +2088,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2258,7 +2096,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2266,7 +2104,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2282,7 +2120,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2290,7 +2128,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2298,7 +2136,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2306,7 +2144,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2330,7 +2168,7 @@
         <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,7 +2176,7 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2385,22 +2223,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -2583,22 +2421,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -2775,22 +2613,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -2800,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2863,22 +2701,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -3039,22 +2877,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -3231,22 +3069,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -3359,22 +3197,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -3455,22 +3293,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>

</xml_diff>

<commit_message>
Merging after IEPD updates to support race code and recidivism date.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Codes.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Codes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="19425" windowHeight="13065" tabRatio="771" firstSheet="1" activeTab="15"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="19425" windowHeight="13065" tabRatio="771" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="OffLevel" sheetId="4" r:id="rId1"/>
@@ -18,11 +18,10 @@
     <sheet name="PleaChange" sheetId="18" r:id="rId9"/>
     <sheet name="ProDispCode" sheetId="20" r:id="rId10"/>
     <sheet name="PTStat" sheetId="21" r:id="rId11"/>
-    <sheet name="Race" sheetId="22" r:id="rId12"/>
-    <sheet name="SentCat" sheetId="25" r:id="rId13"/>
-    <sheet name="VTRes" sheetId="26" r:id="rId14"/>
-    <sheet name="County" sheetId="27" r:id="rId15"/>
-    <sheet name="Sentence" sheetId="28" r:id="rId16"/>
+    <sheet name="SentCat" sheetId="25" r:id="rId12"/>
+    <sheet name="VTRes" sheetId="26" r:id="rId13"/>
+    <sheet name="County" sheetId="27" r:id="rId14"/>
+    <sheet name="Sentence" sheetId="28" r:id="rId15"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="195">
   <si>
     <t>UNKNOWN</t>
   </si>
@@ -345,33 +344,6 @@
     <t>BAIL ORDERED</t>
   </si>
   <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>African American</t>
-  </si>
-  <si>
-    <t>Asian</t>
-  </si>
-  <si>
-    <t>Caucasian</t>
-  </si>
-  <si>
-    <t>Hispanic</t>
-  </si>
-  <si>
-    <t>Native American</t>
-  </si>
-  <si>
-    <t>Not Reported</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Not Known</t>
-  </si>
-  <si>
     <t>DEATH</t>
   </si>
   <si>
@@ -619,12 +591,6 @@
   </si>
   <si>
     <t>Pre-Trial Status code set</t>
-  </si>
-  <si>
-    <t>RaceCode</t>
-  </si>
-  <si>
-    <t>Race code set</t>
   </si>
   <si>
     <t>SentCatCode</t>
@@ -1155,22 +1121,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -1239,22 +1205,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -1359,22 +1325,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -1450,43 +1416,42 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>103</v>
@@ -1494,7 +1459,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>104</v>
@@ -1502,7 +1467,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>105</v>
@@ -1510,7 +1475,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>106</v>
@@ -1518,7 +1483,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>107</v>
@@ -1526,7 +1491,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>108</v>
@@ -1556,11 +1521,206 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
       <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1578,311 +1738,125 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>130</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>66</v>
-      </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>77</v>
-      </c>
-      <c r="B35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>99</v>
-      </c>
-      <c r="B37" t="s">
-        <v>142</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1903,40 +1877,40 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>143</v>
@@ -1944,7 +1918,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>144</v>
@@ -1952,7 +1926,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>145</v>
@@ -1960,7 +1934,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>146</v>
@@ -1968,7 +1942,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>147</v>
@@ -1976,7 +1950,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>148</v>
@@ -1984,7 +1958,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>149</v>
@@ -1992,7 +1966,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>150</v>
@@ -2000,7 +1974,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>151</v>
@@ -2008,16 +1982,48 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" s="9"/>
     </row>
   </sheetData>
@@ -2039,174 +2045,6 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -2217,22 +2055,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -2242,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2250,7 +2088,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2258,7 +2096,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2266,7 +2104,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2282,7 +2120,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2290,7 +2128,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2298,7 +2136,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2306,7 +2144,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2330,7 +2168,7 @@
         <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,7 +2176,7 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2385,22 +2223,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -2583,22 +2421,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -2775,22 +2613,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -2800,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2863,22 +2701,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -3039,22 +2877,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -3231,22 +3069,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -3359,22 +3197,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>
@@ -3455,22 +3293,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="8"/>

</xml_diff>